<commit_message>
Updated mapping and sort order
</commit_message>
<xml_diff>
--- a/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12232 JE 1st dose performance report/43. JE 1st dose performance report.xlsx
+++ b/OutputReports/DHIS2 Reports/HTML Reports/Maharashtra/RCH Reports/#12232 JE 1st dose performance report/43. JE 1st dose performance report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23895" windowHeight="10350"/>
+    <workbookView windowWidth="20385" windowHeight="8370"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,13 +43,13 @@
     <t xml:space="preserve">Progressive </t>
   </si>
   <si>
-    <t>aYkYAjbmDKC.v5em9rXmyXm+ aYkYAjbmDKC.GUNhDhI7FcG</t>
+    <t>aYkYAjbmDKC.v5em9rXmyXm+ aYkYAjbmDKC.GUNhDhI7FcG + RQWW5fNZUtP.v5em9rXmyXm + RQWW5fNZUtP.GUNhDhI7FcG</t>
   </si>
   <si>
     <t>C column's cumulative data (upto that month in financial year)</t>
   </si>
   <si>
-    <t>aYkYAjbmDKC.MkIk8f8jTxz</t>
+    <t>aYkYAjbmDKC.MkIk8f8jTxz + RQWW5fNZUtP.MkIk8f8jTxz</t>
   </si>
   <si>
     <t>E column's cumulative data (upto that month in financial year)</t>
@@ -120,10 +120,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="176" formatCode="_ &quot;₹&quot;\ * #,##0_ ;_ &quot;₹&quot;\ * \-#,##0_ ;_ &quot;₹&quot;\ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="178" formatCode="_ &quot;₹&quot;\ * #,##0.00_ ;_ &quot;₹&quot;\ * \-#,##0.00_ ;_ &quot;₹&quot;\ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -180,21 +180,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -202,6 +187,44 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
@@ -209,31 +232,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -247,37 +256,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="15"/>
       <color theme="3"/>
@@ -286,23 +264,37 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -310,7 +302,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -343,49 +343,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -397,127 +493,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -609,17 +609,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
@@ -645,8 +634,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -684,23 +688,19 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FFB2B2B2"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,152 +709,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="25" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="21" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -884,6 +884,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -1219,7 +1222,7 @@
   <dimension ref="A1:H25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="7"/>
@@ -1299,7 +1302,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" ht="60" spans="1:8">
+    <row r="5" ht="120" spans="1:8">
       <c r="A5" s="9"/>
       <c r="B5" s="9"/>
       <c r="C5" s="10" t="s">
@@ -1308,109 +1311,109 @@
       <c r="D5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="12" t="s">
         <v>11</v>
       </c>
       <c r="F5" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" ht="33.75" spans="4:4">
-      <c r="D7" s="13" t="s">
+      <c r="D7" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="8" spans="4:4">
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="15" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="9" spans="4:4">
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="15" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="4:4">
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="4:4">
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="15" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="12" spans="4:4">
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="4:4">
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="14" spans="4:4">
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="15" spans="4:4">
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="15" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="16" spans="4:4">
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="15" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="17" spans="4:4">
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="15" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="18" spans="4:4">
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="19" spans="4:4">
-      <c r="D19" s="15"/>
+      <c r="D19" s="16"/>
     </row>
     <row r="20" ht="33.75" spans="4:4">
-      <c r="D20" s="13" t="s">
+      <c r="D20" s="14" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="21" spans="4:4">
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="15" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="22" spans="4:4">
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="15" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="4:4">
-      <c r="D23" s="14" t="s">
+      <c r="D23" s="15" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="4:4">
-      <c r="D24" s="14" t="s">
+      <c r="D24" s="15" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="4:4">
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="15" t="s">
         <v>32</v>
       </c>
     </row>

</xml_diff>